<commit_message>
updated localization and channel coordinates
</commit_message>
<xml_diff>
--- a/Localization/CHMap.xlsx
+++ b/Localization/CHMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaosuhu/Documents/MATLAB/PROJECT_BilingualRO1/Code_R01ProjectAnalysis/Localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF40114-6071-EC46-BB7D-F49F0EF0599A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117C3A0-EA91-3146-82FF-039CBBC4F583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{9A346832-1769-1347-B2C3-E100D62226F3}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="33540" windowHeight="21700" activeTab="1" xr2:uid="{9A346832-1769-1347-B2C3-E100D62226F3}"/>
   </bookViews>
   <sheets>
     <sheet name="MRI" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -523,6 +523,8 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1348,7 +1350,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,26 +1408,26 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="9">
         <v>-54.5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="9">
         <v>44</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="9">
         <v>-1.5</v>
       </c>
     </row>
@@ -1452,26 +1454,26 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="9">
         <v>-61</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="9">
         <v>25</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1521,193 +1523,193 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="6">
         <v>-67.5</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="6">
         <v>-7</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>-9</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="6">
         <v>-64.5</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="6">
         <v>-9</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="H9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="6">
         <v>-65</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="6">
         <v>-23.5</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="6">
         <v>-6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <v>-62</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <v>-25.5</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="21">
         <v>-60</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="21">
         <v>-38.5</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="21">
         <v>-3.5</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+    </row>
+    <row r="13" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="21">
         <v>-56.5</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="21">
         <v>-38.5</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="21">
         <v>12.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="21">
         <v>-52</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="21">
         <v>-51.5</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="21">
         <v>-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="21">
         <v>-48.5</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="21">
         <v>-51.5</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="21">
         <v>13</v>
       </c>
     </row>

</xml_diff>